<commit_message>
adding basic schema with test upload
</commit_message>
<xml_diff>
--- a/resources/basic_schema_upload.xlsx
+++ b/resources/basic_schema_upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Internal ID</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Project</t>
   </si>
   <si>
+    <t xml:space="preserve">Files</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHOULD BE DISCARDED</t>
   </si>
   <si>
@@ -74,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">The Planet Bethlehem Archive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eye.jpg</t>
   </si>
 </sst>
 </file>
@@ -88,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -109,6 +116,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -195,7 +203,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.53"/>
@@ -231,34 +239,40 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>